<commit_message>
Add ExcelReader for Products
</commit_message>
<xml_diff>
--- a/src/test/resources/products.xlsx
+++ b/src/test/resources/products.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yharasym\workspace298\lv298\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yharasym\workspace\lv344\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
-  <si>
-    <t>searchKey</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
@@ -39,37 +36,34 @@
     <t>US_DOLLAR</t>
   </si>
   <si>
-    <t>mac</t>
-  </si>
-  <si>
     <t>MacBook</t>
   </si>
   <si>
     <t>Intel Core 2 Duo processor Powered by an Intel Core 2 Duo processor at speeds up to 2.1</t>
   </si>
   <si>
-    <t>560.94</t>
-  </si>
-  <si>
-    <t>487.62</t>
+    <t>472.33</t>
+  </si>
+  <si>
+    <t>368.73</t>
   </si>
   <si>
     <t>602.00</t>
   </si>
   <si>
-    <t>MacBook Air</t>
-  </si>
-  <si>
-    <t>MacBook Air is ultrathin, ultraportable, and ultra unlike anything else. But you don’t lose</t>
-  </si>
-  <si>
-    <t>1,120.02</t>
-  </si>
-  <si>
-    <t>973.62</t>
-  </si>
-  <si>
-    <t>1,202.00</t>
+    <t>iPhone</t>
+  </si>
+  <si>
+    <t>iPhone is a revolutionary new mobile phone that allows you to make a call by simply tapping a nam</t>
+  </si>
+  <si>
+    <t>96.66</t>
+  </si>
+  <si>
+    <t>75.46</t>
+  </si>
+  <si>
+    <t>123.20</t>
   </si>
 </sst>
 </file>
@@ -571,17 +565,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -903,79 +888,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="6" width="15.7109375" style="2" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>